<commit_message>
Changed active cells on test files
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/100_000_rows.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/100_000_rows.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnorantala/Projects/ProTools/SpreadSheet/source/spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svn\GIT\tagetik-2017-spreadsheet-1.4\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-44300" yWindow="2240" windowWidth="31740" windowHeight="21020" tabRatio="500"/>
+    <workbookView xWindow="-44295" yWindow="2235" windowWidth="31740" windowHeight="21015" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,6 +82,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -352,28 +355,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99948" workbookViewId="0">
-      <selection activeCell="A99998" sqref="A99998"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20000" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20000" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20000" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32715" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32715" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32715" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="100000" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100000" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100000" t="s">
         <v>2</v>
       </c>

</xml_diff>